<commit_message>
Completé el informe con cosas del PCB. Falta armar y medir.
</commit_message>
<xml_diff>
--- a/EJ7/Mediciones/Mediciones.xlsx
+++ b/EJ7/Mediciones/Mediciones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Estados</t>
   </si>
@@ -84,13 +84,16 @@
   </si>
   <si>
     <t>Fotos de la implemetación!</t>
+  </si>
+  <si>
+    <t>RECORDAR! Medir en el osciloscopio usando los 4 canales para el clock y cada bit del contador.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +117,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,8 +151,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -273,11 +290,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,6 +372,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -610,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U7"/>
+  <dimension ref="B1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +804,25 @@
         <v>5</v>
       </c>
     </row>
+    <row r="9" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B10:E11"/>
+  </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E7">
       <formula1>$U$2:$U$7</formula1>

</xml_diff>

<commit_message>
Completé las mediciones y las agregué al informe. Redondie y resumí un poco más el informe...
</commit_message>
<xml_diff>
--- a/EJ7/Mediciones/Mediciones.xlsx
+++ b/EJ7/Mediciones/Mediciones.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Estados</t>
   </si>
@@ -83,10 +83,16 @@
     <t>Frec. Máxima.</t>
   </si>
   <si>
-    <t>Fotos de la implemetación!</t>
-  </si>
-  <si>
     <t>RECORDAR! Medir en el osciloscopio usando los 4 canales para el clock y cada bit del contador.</t>
+  </si>
+  <si>
+    <t>Fotos de la implementación!</t>
+  </si>
+  <si>
+    <t>Para el caso sincrónico. La amarilla es la entrada del clock, la verde es Q2, la azul es Q1 y la rosa es Q0. Se tuvo que medir usando Single. Se detecto que las salidas de los flip flops eran de 4V.</t>
+  </si>
+  <si>
+    <t>Mismo caso que los otros del sincrónico, las salidas no llegan a 5 V. Amarilla es clock, verde es Q2, azul es Q1 y luego rosa es Q0.</t>
   </si>
 </sst>
 </file>
@@ -690,7 +696,7 @@
   <dimension ref="B1:U11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,14 +743,14 @@
         <v>13</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3" s="10"/>
       <c r="U3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
@@ -755,14 +761,16 @@
         <v>18</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="U4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
@@ -773,21 +781,23 @@
         <v>18</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="U5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
       <c r="E6" s="11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F6" s="10"/>
       <c r="U6" s="2" t="s">
@@ -807,7 +817,7 @@
     <row r="9" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>

</xml_diff>